<commit_message>
Added capacity to save PQ and ST arrays from ez_rsas.py
</commit_message>
<xml_diff>
--- a/examples/LinearReservoir.xlsx
+++ b/examples/LinearReservoir.xlsx
@@ -240,8 +240,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -317,7 +321,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +355,8 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -384,6 +390,8 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,7 +740,7 @@
   <dimension ref="B6:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -843,7 +851,7 @@
   <dimension ref="A1:K1125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -45922,7 +45930,7 @@
   <dimension ref="A1:B1097"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>